<commit_message>
First draft of 2015 data ready
</commit_message>
<xml_diff>
--- a/Data2015/rawData/NH-for-EPA-2015-cyanoMonDataEntry-addenda.xlsx
+++ b/Data2015/rawData/NH-for-EPA-2015-cyanoMonDataEntry-addenda.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bryan\PortableApps\R\scripts\Reg1Cyano\Data2015\rawData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="19035" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10836"/>
   </bookViews>
   <sheets>
     <sheet name="Field Data Entry" sheetId="2" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Field Data Entry'!$C$1:$AB$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Lab Data Entry'!$A$1:$S$1</definedName>
-    <definedName name="Fa">'Field Data Entry'!$XEP$21</definedName>
+    <definedName name="Fa">'Field Data Entry'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -145,9 +150,6 @@
     <t>commentWB</t>
   </si>
   <si>
-    <t>StationDescription</t>
-  </si>
-  <si>
     <t>stationType</t>
   </si>
   <si>
@@ -227,6 +229,9 @@
   </si>
   <si>
     <t>T. MacConnell</t>
+  </si>
+  <si>
+    <t>stationDescription</t>
   </si>
 </sst>
 </file>
@@ -377,7 +382,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -402,7 +407,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -418,6 +422,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -466,7 +473,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,7 +508,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -710,49 +717,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1048277"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:AB2"/>
+      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="61.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
@@ -784,22 +787,22 @@
         <v>31</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>30</v>
@@ -808,76 +811,72 @@
         <v>29</v>
       </c>
       <c r="S1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>56</v>
-      </c>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="5"/>
-    </row>
-    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>60</v>
-      </c>
-      <c r="H2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" t="s">
-        <v>61</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2">
         <v>-72.042599999999993</v>
@@ -886,7 +885,7 @@
         <v>43.406083000000002</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q2" t="s">
         <v>14</v>
@@ -895,10 +894,10 @@
         <v>42226</v>
       </c>
       <c r="T2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V2" t="s">
         <v>7</v>
@@ -909,296 +908,50 @@
       <c r="AA2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1048277" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L1048277" s="4"/>
-      <c r="O1048277" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:AB1"/>
   <dataValidations count="50">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Were photos taken?" prompt="If photos were taken of the site or the sampling select &quot;Yes&quot;." sqref="AA6:AA1048576 AA2:AA4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Were photos taken?" prompt="If photos were taken of the site or the sampling select &quot;Yes&quot;." sqref="AA2">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Weather Conditions" prompt="Describe the weather conditions as: &quot;Clear&quot;; &quot;Partly Cloudy&quot;; &quot;Overcast&quot;; or &quot;Rain&quot;" sqref="Z6:Z1048576 Z2:Z4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Weather Conditions" prompt="Describe the weather conditions as: &quot;Clear&quot;; &quot;Partly Cloudy&quot;; &quot;Overcast&quot;; or &quot;Rain&quot;" sqref="Z2">
       <formula1>"Clear, Partly Cloudy, Overcast, Rain"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" promptTitle="Water Temperature Centrigrade" prompt="What is the temperature of the sample at time of collection?" sqref="Y6:Y1048576 Y2:Y4">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" promptTitle="Water Temperature Centrigrade" prompt="What is the temperature of the sample at time of collection?" sqref="Y2">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Surface Water Conditions" prompt="Describe the water surfaces as:  &quot;Calm&quot;; &quot;Ripples&quot;; &quot;Choppy&quot;; &amp;  &quot;White Caps&quot;" sqref="X6:X1048576 X2:X4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Sample Depth" prompt="Sample depth in Meters.  This should be 1 (m) for &quot;nearShore&quot; stations and 3 (m) but other depths could be entered if necessary." sqref="W6:W1048576 W2:W4"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Sample Replicate" prompt="Select &quot;primary&quot; or &quot;duplicate&quot;.  For each station and date you can have only one primary sample but many duplicates.  The first sample is the primary and subsequent samples are duplicates." sqref="V6:V1048576 V2:V4">
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Surface Water Conditions" prompt="Describe the water surfaces as:  &quot;Calm&quot;; &quot;Ripples&quot;; &quot;Choppy&quot;; &amp;  &quot;White Caps&quot;" sqref="X2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Sample Depth" prompt="Sample depth in Meters.  This should be 1 (m) for &quot;nearShore&quot; stations and 3 (m) but other depths could be entered if necessary." sqref="W2"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Sample Replicate" prompt="Select &quot;primary&quot; or &quot;duplicate&quot;.  For each station and date you can have only one primary sample but many duplicates.  The first sample is the primary and subsequent samples are duplicates." sqref="V2">
       <formula1>"Primary, Duplicate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Sample Method" prompt="This should  be &quot;Integrated Sampler&quot;; If you used another method select other and then give details in the field &quot;commentSample&quot;" sqref="U6:U1048576 U2:U4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Sample Method" prompt="This should  be &quot;Integrated Sampler&quot;; If you used another method select other and then give details in the field &quot;commentSample&quot;" sqref="U2">
       <formula1>"Intergrated Sampler, Other"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Who collected the sample" prompt="names separated by commas." sqref="T6:T1048576 T2:T4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Time" prompt="When was the sample collected? Use HH:MM AM/PM" sqref="S6:S1048576 S2:S4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Date of Sample" prompt="The date sample was collected" sqref="R6:R1048576 R2:R4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Comments Station" prompt="Add additional information about the station here." sqref="P6:P1048576 P2:P4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Source of Location" prompt="How was the location determined (e.g.,&quot;WaterbodyDatabase&quot;; &quot;GPS&quot;; &quot;GoogleEarth&quot;; &quot;BingMaps&quot;; &quot;topoMap&quot;)?" sqref="O6:O1048576 O2:O4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="latitude of the sample station" prompt="Decimal Degrees with at least 4 (more is better) decimal places.  For New England values should be between 40 and 46 degrees._x000a_" sqref="N6:N1048576 N2:N4"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Station Type" prompt="Choose &quot;nearShore&quot;, &quot;offShore&quot; or &quot;other&quot;. If &quot;other&quot; explain in field &quot;commentStation&quot;" sqref="L6:L1048576 L2:L4">
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Who collected the sample" prompt="names separated by commas." sqref="T2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Time" prompt="When was the sample collected? Use HH:MM AM/PM" sqref="S2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Date of Sample" prompt="The date sample was collected" sqref="R2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Comments Station" prompt="Add additional information about the station here." sqref="P2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Source of Location" prompt="How was the location determined (e.g.,&quot;WaterbodyDatabase&quot;; &quot;GPS&quot;; &quot;GoogleEarth&quot;; &quot;BingMaps&quot;; &quot;topoMap&quot;)?" sqref="O2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="latitude of the sample station" prompt="Decimal Degrees with at least 4 (more is better) decimal places.  For New England values should be between 40 and 46 degrees._x000a_" sqref="N2"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Station Type" prompt="Choose &quot;nearShore&quot;, &quot;offShore&quot; or &quot;other&quot;. If &quot;other&quot; explain in field &quot;commentStation&quot;" sqref="L2">
       <formula1>"nearShore, offShore, other"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Waterbody Comments" prompt="Add additional information about the waterbody here." sqref="I6:I1048576 I2:I4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Nearest Town" prompt="input the name of the closest town to the lake." sqref="H6:H1048576 H2:H4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="State" prompt="Use the standard 2 letter abbreviation" sqref="G6:G1048576 G2:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Acronym for the organization" prompt="Current Choices: AED, CRWA, CTDEEP, MEDEP, NHDES, RIWW, UNH, VTDEC" sqref="A6:A1048576 A1:A4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contact Name" prompt="Who is responsible for the data?" sqref="B6:B1048576 B1:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Email Address" prompt="of the contact person." sqref="C6:C1048576 C1:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phone Number" prompt="of the contact person.  xxx-xxx-xxxx" sqref="D6:D1048576 D1:D4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Waterbody Name" prompt="with no abbreviations.  Check spelling and try to be consistent." sqref="F6:F1048576 F1:F4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Unique ID for the waterbody" prompt="If your organzation has a unique identifier for the waterbody use it here.  If not use your orgID followed by an underscore and a unique three digit  number. (e.g. UNH_001)" sqref="E6:E1048576 E1:E4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Sample ID" prompt="Assign a unique ID to the analysis.  Unique means unique to the waterbody and date. Could be  &quot;Samp&quot; and a two digit sequential number (e.g., Samp01, Samp02 etc.)" sqref="Q6:Q1048576 Q2:Q4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Longitude of the Station" prompt="Longitude should be in decimal degrees with at least 4 (more is better) decimal places.  For New England longitude will be between -69 and -81 degrees." sqref="M6:M1048576 M2:M4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Station Description" prompt="Brief description of where the station is." sqref="K6:K1048576 K2:K4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Unique ID for the Station" prompt="If your organzation has a unique identifier for the station use it here. Unique means unique to this waterbody.  If not use &quot;Sta&quot; followed by a unique two digit  number.  (e.g. Sta01, Sta02, etc)." sqref="J6:J1048576 J2:J4"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Waterbody Comments" prompt="Add additional information about the waterbody here." sqref="I2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Nearest Town" prompt="input the name of the closest town to the lake." sqref="H2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="State" prompt="Use the standard 2 letter abbreviation" sqref="G2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Acronym for the organization" prompt="Current Choices: AED, CRWA, CTDEEP, MEDEP, NHDES, RIWW, UNH, VTDEC" sqref="A1:A2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Contact Name" prompt="Who is responsible for the data?" sqref="B1:B2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Email Address" prompt="of the contact person." sqref="C1:C2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phone Number" prompt="of the contact person.  xxx-xxx-xxxx" sqref="D1:D2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Waterbody Name" prompt="with no abbreviations.  Check spelling and try to be consistent." sqref="F1:F2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Unique ID for the waterbody" prompt="If your organzation has a unique identifier for the waterbody use it here.  If not use your orgID followed by an underscore and a unique three digit  number. (e.g. UNH_001)" sqref="E1:E2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Sample ID" prompt="Assign a unique ID to the analysis.  Unique means unique to the waterbody and date. Could be  &quot;Samp&quot; and a two digit sequential number (e.g., Samp01, Samp02 etc.)" sqref="Q2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Longitude of the Station" prompt="Longitude should be in decimal degrees with at least 4 (more is better) decimal places.  For New England longitude will be between -69 and -81 degrees." sqref="M2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Station Description" prompt="Brief description of where the station is." sqref="K2"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Unique ID for the Station" prompt="If your organzation has a unique identifier for the station use it here. Unique means unique to this waterbody.  If not use &quot;Sta&quot; followed by a unique two digit  number.  (e.g. Sta01, Sta02, etc)." sqref="J2"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Station Type" prompt="Choose &quot;nearShore&quot;, &quot;offShore&quot; or &quot;other&quot;. If &quot;other&quot; explain in field &quot;commentStation&quot;" sqref="L1">
       <formula1>"nearShore, offShore, other"</formula1>
     </dataValidation>
@@ -1256,34 +1009,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>32</v>
       </c>
@@ -1338,7 +1091,7 @@
       <c r="R1" s="6"/>
       <c r="S1" s="5"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1388,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1438,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1488,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1538,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1588,7 +1341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1638,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1688,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>

</xml_diff>